<commit_message>
More results added and work on the code gen and results sections
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Scalability" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="64">
   <si>
     <t>Trial 1</t>
   </si>
@@ -133,6 +133,81 @@
   </si>
   <si>
     <t>Memory</t>
+  </si>
+  <si>
+    <t>SL 1</t>
+  </si>
+  <si>
+    <t>SL 2</t>
+  </si>
+  <si>
+    <t>SL 3</t>
+  </si>
+  <si>
+    <t>SL 4</t>
+  </si>
+  <si>
+    <t>SL 5</t>
+  </si>
+  <si>
+    <t>SL 6</t>
+  </si>
+  <si>
+    <t>SL 7</t>
+  </si>
+  <si>
+    <t>SL 8</t>
+  </si>
+  <si>
+    <t>SL 9</t>
+  </si>
+  <si>
+    <t>SL 10</t>
+  </si>
+  <si>
+    <t>PH 1</t>
+  </si>
+  <si>
+    <t>PH 2</t>
+  </si>
+  <si>
+    <t>PH 3</t>
+  </si>
+  <si>
+    <t>PH 4</t>
+  </si>
+  <si>
+    <t>PH 5</t>
+  </si>
+  <si>
+    <t>PH 6</t>
+  </si>
+  <si>
+    <t>PH 7</t>
+  </si>
+  <si>
+    <t>PH 8</t>
+  </si>
+  <si>
+    <t>PH 9</t>
+  </si>
+  <si>
+    <t>PH 10</t>
+  </si>
+  <si>
+    <t>TTS</t>
+  </si>
+  <si>
+    <t>NHC</t>
+  </si>
+  <si>
+    <t>WH</t>
+  </si>
+  <si>
+    <t>MTG</t>
+  </si>
+  <si>
+    <t>NP</t>
   </si>
 </sst>
 </file>
@@ -693,8 +768,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="182277272"/>
-        <c:axId val="182276880"/>
+        <c:axId val="265353088"/>
+        <c:axId val="265410272"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1117,14 +1192,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="182275704"/>
-        <c:axId val="182276096"/>
+        <c:axId val="265422304"/>
+        <c:axId val="265411680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="182277272"/>
+        <c:axId val="265353088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1000"/>
+          <c:max val="2000"/>
           <c:min val="33"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1236,13 +1311,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="182276880"/>
+        <c:crossAx val="265410272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="297"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="182276880"/>
+        <c:axId val="265410272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1360,12 +1435,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="182277272"/>
+        <c:crossAx val="265353088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="182276096"/>
+        <c:axId val="265411680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1464,12 +1539,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="182275704"/>
+        <c:crossAx val="265422304"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="182275704"/>
+        <c:axId val="265422304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1479,7 +1554,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182276096"/>
+        <c:crossAx val="265411680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2408,8 +2483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5243,43 +5318,217 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:AB6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>35</v>
       </c>
       <c r="C1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>48</v>
+      </c>
+      <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U1" t="s">
+        <v>51</v>
+      </c>
+      <c r="V1" t="s">
+        <v>52</v>
+      </c>
+      <c r="W1" t="s">
+        <v>53</v>
+      </c>
+      <c r="X1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>59</v>
+      </c>
+      <c r="B2" t="e">
+        <f>AVERAGE(H2:Q2)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C2" t="e">
+        <f>AVERAGE(S2:AB2)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B5" si="0">AVERAGE(H3:Q3)</f>
+        <v>31476.799999999999</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C5" si="1">AVERAGE(S3:AB3)</f>
+        <v>713.4</v>
+      </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>31717</v>
+      </c>
+      <c r="I3">
+        <v>31548</v>
+      </c>
+      <c r="J3">
+        <v>31389</v>
+      </c>
+      <c r="K3">
+        <v>31221</v>
+      </c>
+      <c r="L3">
+        <v>31595</v>
+      </c>
+      <c r="M3">
+        <v>31288</v>
+      </c>
+      <c r="N3">
+        <v>31576</v>
+      </c>
+      <c r="O3">
+        <v>31467</v>
+      </c>
+      <c r="P3">
+        <v>31612</v>
+      </c>
+      <c r="Q3">
+        <v>31355</v>
+      </c>
+      <c r="S3">
+        <v>749</v>
+      </c>
+      <c r="T3">
+        <v>718</v>
+      </c>
+      <c r="U3">
+        <v>702</v>
+      </c>
+      <c r="V3">
+        <v>719</v>
+      </c>
+      <c r="W3">
+        <v>718</v>
+      </c>
+      <c r="X3">
+        <v>702</v>
+      </c>
+      <c r="Y3">
+        <v>718</v>
+      </c>
+      <c r="Z3">
+        <v>702</v>
+      </c>
+      <c r="AA3">
+        <v>702</v>
+      </c>
+      <c r="AB3">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C4" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="E5" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" t="e">
+        <f>AVERAGE(H6:Q6)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C6" t="e">
+        <f>AVERAGE(S6:AB6)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New results using proper ode1 for simulink
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Scalability" sheetId="1" r:id="rId1"/>
@@ -281,7 +281,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1161,11 +1160,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="269151784"/>
-        <c:axId val="269151392"/>
+        <c:axId val="213756752"/>
+        <c:axId val="213775464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="269151784"/>
+        <c:axId val="213756752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2000"/>
@@ -1213,7 +1212,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1280,13 +1278,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="269151392"/>
+        <c:crossAx val="213775464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="297"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="269151392"/>
+        <c:axId val="213775464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1337,7 +1335,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1404,7 +1401,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="269151784"/>
+        <c:crossAx val="213756752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2333,8 +2330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2433,7 +2430,7 @@
         <v>0.73199999999999998</v>
       </c>
       <c r="E2">
-        <f>A2*$B$76/1024/1024</f>
+        <f t="shared" ref="E2:E33" si="0">A2*$B$76/1024/1024</f>
         <v>1.094696044921875</v>
       </c>
       <c r="G2">
@@ -2502,15 +2499,15 @@
         <v>66</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B61" si="0">AVERAGE(G3:P3)</f>
+        <f t="shared" ref="B3:B61" si="1">AVERAGE(G3:P3)</f>
         <v>42.652999999999999</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C61" si="1">AVERAGE(R3:AA3)</f>
+        <f t="shared" ref="C3:C61" si="2">AVERAGE(R3:AA3)</f>
         <v>1.7189999999999994</v>
       </c>
       <c r="E3">
-        <f>A3*$B$76/1024/1024</f>
+        <f t="shared" si="0"/>
         <v>2.18939208984375</v>
       </c>
       <c r="G3">
@@ -2579,15 +2576,15 @@
         <v>99</v>
       </c>
       <c r="B4">
+        <f t="shared" si="1"/>
+        <v>77.402999999999992</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="2"/>
+        <v>2.8380000000000005</v>
+      </c>
+      <c r="E4">
         <f t="shared" si="0"/>
-        <v>77.402999999999992</v>
-      </c>
-      <c r="C4">
-        <f t="shared" si="1"/>
-        <v>2.8380000000000005</v>
-      </c>
-      <c r="E4">
-        <f>A4*$B$76/1024/1024</f>
         <v>3.284088134765625</v>
       </c>
       <c r="G4">
@@ -2656,15 +2653,15 @@
         <v>132</v>
       </c>
       <c r="B5">
+        <f t="shared" si="1"/>
+        <v>114.68600000000001</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="2"/>
+        <v>4.6160000000000014</v>
+      </c>
+      <c r="E5">
         <f t="shared" si="0"/>
-        <v>114.68600000000001</v>
-      </c>
-      <c r="C5">
-        <f t="shared" si="1"/>
-        <v>4.6160000000000014</v>
-      </c>
-      <c r="E5">
-        <f>A5*$B$76/1024/1024</f>
         <v>4.3787841796875</v>
       </c>
       <c r="G5">
@@ -2733,15 +2730,15 @@
         <v>165</v>
       </c>
       <c r="B6">
+        <f t="shared" si="1"/>
+        <v>146.36799999999999</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="2"/>
+        <v>7.2849999999999993</v>
+      </c>
+      <c r="E6">
         <f t="shared" si="0"/>
-        <v>146.36799999999999</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="1"/>
-        <v>7.2849999999999993</v>
-      </c>
-      <c r="E6">
-        <f>A6*$B$76/1024/1024</f>
         <v>5.473480224609375</v>
       </c>
       <c r="G6">
@@ -2810,15 +2807,15 @@
         <v>198</v>
       </c>
       <c r="B7">
+        <f t="shared" si="1"/>
+        <v>186.39600000000002</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="2"/>
+        <v>11.095000000000001</v>
+      </c>
+      <c r="E7">
         <f t="shared" si="0"/>
-        <v>186.39600000000002</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="1"/>
-        <v>11.095000000000001</v>
-      </c>
-      <c r="E7">
-        <f>A7*$B$76/1024/1024</f>
         <v>6.56817626953125</v>
       </c>
       <c r="G7">
@@ -2887,15 +2884,15 @@
         <v>231</v>
       </c>
       <c r="B8">
+        <f t="shared" si="1"/>
+        <v>224.20500000000001</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="2"/>
+        <v>16.411999999999999</v>
+      </c>
+      <c r="E8">
         <f t="shared" si="0"/>
-        <v>224.20500000000001</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="1"/>
-        <v>16.411999999999999</v>
-      </c>
-      <c r="E8">
-        <f>A8*$B$76/1024/1024</f>
         <v>7.662872314453125</v>
       </c>
       <c r="G8">
@@ -2964,15 +2961,15 @@
         <v>264</v>
       </c>
       <c r="B9">
+        <f t="shared" si="1"/>
+        <v>258.11800000000005</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="2"/>
+        <v>23.025000000000002</v>
+      </c>
+      <c r="E9">
         <f t="shared" si="0"/>
-        <v>258.11800000000005</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="1"/>
-        <v>23.025000000000002</v>
-      </c>
-      <c r="E9">
-        <f>A9*$B$76/1024/1024</f>
         <v>8.757568359375</v>
       </c>
       <c r="G9">
@@ -3041,15 +3038,15 @@
         <v>297</v>
       </c>
       <c r="B10">
+        <f t="shared" si="1"/>
+        <v>292.83600000000007</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="2"/>
+        <v>31.122999999999998</v>
+      </c>
+      <c r="E10">
         <f t="shared" si="0"/>
-        <v>292.83600000000007</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="1"/>
-        <v>31.122999999999998</v>
-      </c>
-      <c r="E10">
-        <f>A10*$B$76/1024/1024</f>
         <v>9.852264404296875</v>
       </c>
       <c r="G10">
@@ -3118,15 +3115,15 @@
         <v>330</v>
       </c>
       <c r="B11" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="2"/>
+        <v>38.424999999999997</v>
+      </c>
+      <c r="E11">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="1"/>
-        <v>38.424999999999997</v>
-      </c>
-      <c r="E11">
-        <f>A11*$B$76/1024/1024</f>
         <v>10.94696044921875</v>
       </c>
       <c r="R11">
@@ -3165,15 +3162,15 @@
         <v>363</v>
       </c>
       <c r="B12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="2"/>
+        <v>45.940999999999995</v>
+      </c>
+      <c r="E12">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="1"/>
-        <v>45.940999999999995</v>
-      </c>
-      <c r="E12">
-        <f>A12*$B$76/1024/1024</f>
         <v>12.041656494140625</v>
       </c>
       <c r="R12">
@@ -3212,15 +3209,15 @@
         <v>396</v>
       </c>
       <c r="B13" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="2"/>
+        <v>52.601999999999997</v>
+      </c>
+      <c r="E13">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="1"/>
-        <v>52.601999999999997</v>
-      </c>
-      <c r="E13">
-        <f>A13*$B$76/1024/1024</f>
         <v>13.1363525390625</v>
       </c>
       <c r="R13">
@@ -3259,15 +3256,15 @@
         <v>429</v>
       </c>
       <c r="B14" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="2"/>
+        <v>59.35799999999999</v>
+      </c>
+      <c r="E14">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="1"/>
-        <v>59.35799999999999</v>
-      </c>
-      <c r="E14">
-        <f>A14*$B$76/1024/1024</f>
         <v>14.231048583984375</v>
       </c>
       <c r="R14">
@@ -3306,15 +3303,15 @@
         <v>462</v>
       </c>
       <c r="B15" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="2"/>
+        <v>65.38000000000001</v>
+      </c>
+      <c r="E15">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="1"/>
-        <v>65.38000000000001</v>
-      </c>
-      <c r="E15">
-        <f>A15*$B$76/1024/1024</f>
         <v>15.32574462890625</v>
       </c>
       <c r="R15">
@@ -3353,15 +3350,15 @@
         <v>495</v>
       </c>
       <c r="B16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="2"/>
+        <v>71.759999999999991</v>
+      </c>
+      <c r="E16">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="1"/>
-        <v>71.759999999999991</v>
-      </c>
-      <c r="E16">
-        <f>A16*$B$76/1024/1024</f>
         <v>16.420440673828125</v>
       </c>
       <c r="R16">
@@ -3400,15 +3397,15 @@
         <v>528</v>
       </c>
       <c r="B17" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="2"/>
+        <v>77.626000000000005</v>
+      </c>
+      <c r="E17">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="1"/>
-        <v>77.626000000000005</v>
-      </c>
-      <c r="E17">
-        <f>A17*$B$76/1024/1024</f>
         <v>17.51513671875</v>
       </c>
       <c r="R17">
@@ -3447,15 +3444,15 @@
         <v>561</v>
       </c>
       <c r="B18" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="2"/>
+        <v>81.759</v>
+      </c>
+      <c r="E18">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="1"/>
-        <v>81.759</v>
-      </c>
-      <c r="E18">
-        <f>A18*$B$76/1024/1024</f>
         <v>18.609832763671875</v>
       </c>
       <c r="R18">
@@ -3494,15 +3491,15 @@
         <v>594</v>
       </c>
       <c r="B19" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="2"/>
+        <v>84.864000000000019</v>
+      </c>
+      <c r="E19">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="1"/>
-        <v>84.864000000000019</v>
-      </c>
-      <c r="E19">
-        <f>A19*$B$76/1024/1024</f>
         <v>19.70452880859375</v>
       </c>
       <c r="R19">
@@ -3541,15 +3538,15 @@
         <v>627</v>
       </c>
       <c r="B20" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="2"/>
+        <v>91.266999999999996</v>
+      </c>
+      <c r="E20">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="1"/>
-        <v>91.266999999999996</v>
-      </c>
-      <c r="E20">
-        <f>A20*$B$76/1024/1024</f>
         <v>20.799224853515625</v>
       </c>
       <c r="R20">
@@ -3588,15 +3585,15 @@
         <v>660</v>
       </c>
       <c r="B21" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="2"/>
+        <v>96.097999999999999</v>
+      </c>
+      <c r="E21">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="1"/>
-        <v>96.097999999999999</v>
-      </c>
-      <c r="E21">
-        <f>A21*$B$76/1024/1024</f>
         <v>21.8939208984375</v>
       </c>
       <c r="R21">
@@ -3635,15 +3632,15 @@
         <v>693</v>
       </c>
       <c r="B22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="2"/>
+        <v>100.40200000000002</v>
+      </c>
+      <c r="E22">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="1"/>
-        <v>100.40200000000002</v>
-      </c>
-      <c r="E22">
-        <f>A22*$B$76/1024/1024</f>
         <v>22.988616943359375</v>
       </c>
       <c r="R22">
@@ -3682,15 +3679,15 @@
         <v>726</v>
       </c>
       <c r="B23" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="2"/>
+        <v>104.66100000000002</v>
+      </c>
+      <c r="E23">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C23">
-        <f t="shared" si="1"/>
-        <v>104.66100000000002</v>
-      </c>
-      <c r="E23">
-        <f>A23*$B$76/1024/1024</f>
         <v>24.08331298828125</v>
       </c>
       <c r="R23">
@@ -3729,15 +3726,15 @@
         <v>759</v>
       </c>
       <c r="B24" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="2"/>
+        <v>112.742</v>
+      </c>
+      <c r="E24">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C24">
-        <f t="shared" si="1"/>
-        <v>112.742</v>
-      </c>
-      <c r="E24">
-        <f>A24*$B$76/1024/1024</f>
         <v>25.178009033203125</v>
       </c>
       <c r="R24">
@@ -3776,15 +3773,15 @@
         <v>792</v>
       </c>
       <c r="B25" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="2"/>
+        <v>118.29400000000001</v>
+      </c>
+      <c r="E25">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="1"/>
-        <v>118.29400000000001</v>
-      </c>
-      <c r="E25">
-        <f>A25*$B$76/1024/1024</f>
         <v>26.272705078125</v>
       </c>
       <c r="R25">
@@ -3823,15 +3820,15 @@
         <v>825</v>
       </c>
       <c r="B26" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="2"/>
+        <v>121.571</v>
+      </c>
+      <c r="E26">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="1"/>
-        <v>121.571</v>
-      </c>
-      <c r="E26">
-        <f>A26*$B$76/1024/1024</f>
         <v>27.367401123046875</v>
       </c>
       <c r="R26">
@@ -3870,15 +3867,15 @@
         <v>858</v>
       </c>
       <c r="B27" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="2"/>
+        <v>127.53000000000002</v>
+      </c>
+      <c r="E27">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C27">
-        <f t="shared" si="1"/>
-        <v>127.53000000000002</v>
-      </c>
-      <c r="E27">
-        <f>A27*$B$76/1024/1024</f>
         <v>28.46209716796875</v>
       </c>
       <c r="R27">
@@ -3917,15 +3914,15 @@
         <v>891</v>
       </c>
       <c r="B28" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="2"/>
+        <v>131.96099999999998</v>
+      </c>
+      <c r="E28">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C28">
-        <f t="shared" si="1"/>
-        <v>131.96099999999998</v>
-      </c>
-      <c r="E28">
-        <f>A28*$B$76/1024/1024</f>
         <v>29.556793212890625</v>
       </c>
       <c r="R28">
@@ -3964,15 +3961,15 @@
         <v>924</v>
       </c>
       <c r="B29" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="2"/>
+        <v>139.089</v>
+      </c>
+      <c r="E29">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C29">
-        <f t="shared" si="1"/>
-        <v>139.089</v>
-      </c>
-      <c r="E29">
-        <f>A29*$B$76/1024/1024</f>
         <v>30.6514892578125</v>
       </c>
       <c r="R29">
@@ -4011,15 +4008,15 @@
         <v>957</v>
       </c>
       <c r="B30" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="2"/>
+        <v>146.16999999999999</v>
+      </c>
+      <c r="E30">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C30">
-        <f t="shared" si="1"/>
-        <v>146.16999999999999</v>
-      </c>
-      <c r="E30">
-        <f>A30*$B$76/1024/1024</f>
         <v>31.746185302734375</v>
       </c>
       <c r="R30">
@@ -4058,15 +4055,15 @@
         <v>990</v>
       </c>
       <c r="B31" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="2"/>
+        <v>148.38600000000002</v>
+      </c>
+      <c r="E31">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C31">
-        <f t="shared" si="1"/>
-        <v>148.38600000000002</v>
-      </c>
-      <c r="E31">
-        <f>A31*$B$76/1024/1024</f>
         <v>32.84088134765625</v>
       </c>
       <c r="R31">
@@ -4105,15 +4102,15 @@
         <v>1023</v>
       </c>
       <c r="B32" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="2"/>
+        <v>165.96800000000002</v>
+      </c>
+      <c r="E32">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C32">
-        <f t="shared" si="1"/>
-        <v>165.96800000000002</v>
-      </c>
-      <c r="E32">
-        <f>A32*$B$76/1024/1024</f>
         <v>33.935577392578125</v>
       </c>
       <c r="R32">
@@ -4152,15 +4149,15 @@
         <v>1056</v>
       </c>
       <c r="B33" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="2"/>
+        <v>166.64600000000002</v>
+      </c>
+      <c r="E33">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C33">
-        <f t="shared" si="1"/>
-        <v>166.64600000000002</v>
-      </c>
-      <c r="E33">
-        <f>A33*$B$76/1024/1024</f>
         <v>35.0302734375</v>
       </c>
       <c r="R33">
@@ -4199,15 +4196,15 @@
         <v>1089</v>
       </c>
       <c r="B34" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>170.52499999999998</v>
       </c>
       <c r="E34">
-        <f>A34*$B$76/1024/1024</f>
+        <f t="shared" ref="E34:E61" si="3">A34*$B$76/1024/1024</f>
         <v>36.124969482421875</v>
       </c>
       <c r="R34">
@@ -4246,15 +4243,15 @@
         <v>1122</v>
       </c>
       <c r="B35" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>172.89400000000001</v>
       </c>
       <c r="E35">
-        <f>A35*$B$76/1024/1024</f>
+        <f t="shared" si="3"/>
         <v>37.21966552734375</v>
       </c>
       <c r="R35">
@@ -4293,15 +4290,15 @@
         <v>1155</v>
       </c>
       <c r="B36" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>184.298</v>
       </c>
       <c r="E36">
-        <f>A36*$B$76/1024/1024</f>
+        <f t="shared" si="3"/>
         <v>38.314361572265625</v>
       </c>
       <c r="R36">
@@ -4340,15 +4337,15 @@
         <v>1188</v>
       </c>
       <c r="B37" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>182.97199999999998</v>
       </c>
       <c r="E37">
-        <f>A37*$B$76/1024/1024</f>
+        <f t="shared" si="3"/>
         <v>39.4090576171875</v>
       </c>
       <c r="R37">
@@ -4387,15 +4384,15 @@
         <v>1221</v>
       </c>
       <c r="B38" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>194.17299999999997</v>
       </c>
       <c r="E38">
-        <f>A38*$B$76/1024/1024</f>
+        <f t="shared" si="3"/>
         <v>40.503753662109375</v>
       </c>
       <c r="R38">
@@ -4434,15 +4431,15 @@
         <v>1254</v>
       </c>
       <c r="B39" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>206.45100000000002</v>
       </c>
       <c r="E39">
-        <f>A39*$B$76/1024/1024</f>
+        <f t="shared" si="3"/>
         <v>41.59844970703125</v>
       </c>
       <c r="R39">
@@ -4481,15 +4478,15 @@
         <v>1287</v>
       </c>
       <c r="B40" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>224.84299999999999</v>
       </c>
       <c r="E40">
-        <f>A40*$B$76/1024/1024</f>
+        <f t="shared" si="3"/>
         <v>42.693145751953125</v>
       </c>
       <c r="R40">
@@ -4528,15 +4525,15 @@
         <v>1320</v>
       </c>
       <c r="B41" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>219.429</v>
       </c>
       <c r="E41">
-        <f>A41*$B$76/1024/1024</f>
+        <f t="shared" si="3"/>
         <v>43.787841796875</v>
       </c>
       <c r="R41">
@@ -4575,15 +4572,15 @@
         <v>1353</v>
       </c>
       <c r="B42" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>232.77699999999996</v>
       </c>
       <c r="E42">
-        <f>A42*$B$76/1024/1024</f>
+        <f t="shared" si="3"/>
         <v>44.882537841796875</v>
       </c>
       <c r="R42">
@@ -4622,15 +4619,15 @@
         <v>1386</v>
       </c>
       <c r="B43" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>246.34100000000004</v>
       </c>
       <c r="E43">
-        <f>A43*$B$76/1024/1024</f>
+        <f t="shared" si="3"/>
         <v>45.97723388671875</v>
       </c>
       <c r="R43">
@@ -4669,15 +4666,15 @@
         <v>1419</v>
       </c>
       <c r="B44" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>256.27499999999998</v>
       </c>
       <c r="E44">
-        <f>A44*$B$76/1024/1024</f>
+        <f t="shared" si="3"/>
         <v>47.071929931640625</v>
       </c>
       <c r="R44">
@@ -4716,15 +4713,15 @@
         <v>1452</v>
       </c>
       <c r="B45" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>273.5</v>
       </c>
       <c r="E45">
-        <f>A45*$B$76/1024/1024</f>
+        <f t="shared" si="3"/>
         <v>48.1666259765625</v>
       </c>
       <c r="R45">
@@ -4763,15 +4760,15 @@
         <v>1485</v>
       </c>
       <c r="B46" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>268.46000000000004</v>
       </c>
       <c r="E46">
-        <f>A46*$B$76/1024/1024</f>
+        <f t="shared" si="3"/>
         <v>49.261322021484375</v>
       </c>
       <c r="R46">
@@ -4810,15 +4807,15 @@
         <v>1518</v>
       </c>
       <c r="B47" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>296.25999999999993</v>
       </c>
       <c r="E47">
-        <f>A47*$B$76/1024/1024</f>
+        <f t="shared" si="3"/>
         <v>50.35601806640625</v>
       </c>
       <c r="R47">
@@ -4857,15 +4854,15 @@
         <v>1551</v>
       </c>
       <c r="B48" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>304.48099999999999</v>
       </c>
       <c r="E48">
-        <f>A48*$B$76/1024/1024</f>
+        <f t="shared" si="3"/>
         <v>51.450714111328125</v>
       </c>
       <c r="R48">
@@ -4904,15 +4901,15 @@
         <v>1584</v>
       </c>
       <c r="B49" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>328.75600000000003</v>
       </c>
       <c r="E49">
-        <f>A49*$B$76/1024/1024</f>
+        <f t="shared" si="3"/>
         <v>52.54541015625</v>
       </c>
       <c r="R49">
@@ -4951,15 +4948,15 @@
         <v>1617</v>
       </c>
       <c r="B50" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>341.89</v>
       </c>
       <c r="E50">
-        <f>A50*$B$76/1024/1024</f>
+        <f t="shared" si="3"/>
         <v>53.640106201171875</v>
       </c>
       <c r="R50">
@@ -4998,15 +4995,15 @@
         <v>1650</v>
       </c>
       <c r="B51" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>383.59</v>
       </c>
       <c r="E51">
-        <f>A51*$B$76/1024/1024</f>
+        <f t="shared" si="3"/>
         <v>54.73480224609375</v>
       </c>
       <c r="R51">
@@ -5045,15 +5042,15 @@
         <v>1683</v>
       </c>
       <c r="B52" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>390.31299999999999</v>
       </c>
       <c r="E52">
-        <f>A52*$B$76/1024/1024</f>
+        <f t="shared" si="3"/>
         <v>55.829498291015625</v>
       </c>
       <c r="R52">
@@ -5092,15 +5089,15 @@
         <v>1716</v>
       </c>
       <c r="B53" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>395.11700000000008</v>
       </c>
       <c r="E53">
-        <f>A53*$B$76/1024/1024</f>
+        <f t="shared" si="3"/>
         <v>56.9241943359375</v>
       </c>
       <c r="R53">
@@ -5139,15 +5136,15 @@
         <v>1749</v>
       </c>
       <c r="B54" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>436.78800000000001</v>
       </c>
       <c r="E54">
-        <f>A54*$B$76/1024/1024</f>
+        <f t="shared" si="3"/>
         <v>58.018890380859375</v>
       </c>
       <c r="R54">
@@ -5186,15 +5183,15 @@
         <v>1782</v>
       </c>
       <c r="B55" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>487.471</v>
       </c>
       <c r="E55">
-        <f>A55*$B$76/1024/1024</f>
+        <f t="shared" si="3"/>
         <v>59.11358642578125</v>
       </c>
       <c r="R55">
@@ -5233,15 +5230,15 @@
         <v>1815</v>
       </c>
       <c r="B56" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>476.83000000000004</v>
       </c>
       <c r="E56">
-        <f>A56*$B$76/1024/1024</f>
+        <f t="shared" si="3"/>
         <v>60.208282470703125</v>
       </c>
       <c r="R56">
@@ -5280,15 +5277,15 @@
         <v>1848</v>
       </c>
       <c r="B57" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>485.89299999999992</v>
       </c>
       <c r="E57">
-        <f>A57*$B$76/1024/1024</f>
+        <f t="shared" si="3"/>
         <v>61.302978515625</v>
       </c>
       <c r="R57">
@@ -5327,15 +5324,15 @@
         <v>1881</v>
       </c>
       <c r="B58" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>537.22299999999996</v>
       </c>
       <c r="E58">
-        <f>A58*$B$76/1024/1024</f>
+        <f t="shared" si="3"/>
         <v>62.397674560546875</v>
       </c>
       <c r="R58">
@@ -5374,15 +5371,15 @@
         <v>1914</v>
       </c>
       <c r="B59" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>543.78600000000006</v>
       </c>
       <c r="E59">
-        <f>A59*$B$76/1024/1024</f>
+        <f t="shared" si="3"/>
         <v>63.49237060546875</v>
       </c>
       <c r="R59">
@@ -5421,15 +5418,15 @@
         <v>1947</v>
       </c>
       <c r="B60" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>564.42499999999995</v>
       </c>
       <c r="E60">
-        <f>A60*$B$76/1024/1024</f>
+        <f t="shared" si="3"/>
         <v>64.587066650390625</v>
       </c>
       <c r="R60">
@@ -5468,15 +5465,15 @@
         <v>1980</v>
       </c>
       <c r="B61" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>608.72700000000009</v>
       </c>
       <c r="E61">
-        <f>A61*$B$76/1024/1024</f>
+        <f t="shared" si="3"/>
         <v>65.6817626953125</v>
       </c>
       <c r="R61">
@@ -5741,8 +5738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5837,7 +5834,7 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B5" si="0">AVERAGE(H3:Q3)</f>
-        <v>31476.799999999999</v>
+        <v>14253.6</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C5" si="1">AVERAGE(S3:AB3)</f>
@@ -5847,34 +5844,34 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>31717</v>
+        <v>14418</v>
       </c>
       <c r="I3">
-        <v>31548</v>
+        <v>14271</v>
       </c>
       <c r="J3">
-        <v>31389</v>
+        <v>14266</v>
       </c>
       <c r="K3">
-        <v>31221</v>
+        <v>14235</v>
       </c>
       <c r="L3">
-        <v>31595</v>
+        <v>14279</v>
       </c>
       <c r="M3">
-        <v>31288</v>
+        <v>14219</v>
       </c>
       <c r="N3">
-        <v>31576</v>
+        <v>14260</v>
       </c>
       <c r="O3">
-        <v>31467</v>
+        <v>14205</v>
       </c>
       <c r="P3">
-        <v>31612</v>
+        <v>14201</v>
       </c>
       <c r="Q3">
-        <v>31355</v>
+        <v>14182</v>
       </c>
       <c r="S3">
         <v>749</v>

</xml_diff>

<commit_message>
Added Train-Gate Piha code and results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Scalability" sheetId="1" r:id="rId1"/>
     <sheet name="Simulation Time" sheetId="2" r:id="rId2"/>
-    <sheet name="Executable Size" sheetId="3" r:id="rId3"/>
+    <sheet name="Memory Usage" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="52">
   <si>
     <t># Cells</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>Piha</t>
-  </si>
-  <si>
-    <t>Heart</t>
   </si>
   <si>
     <t>SL 1</t>
@@ -281,7 +278,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1161,11 +1157,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="289031360"/>
-        <c:axId val="371191704"/>
+        <c:axId val="288222616"/>
+        <c:axId val="288763384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="289031360"/>
+        <c:axId val="288222616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2000"/>
@@ -1213,7 +1209,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1280,13 +1275,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="371191704"/>
+        <c:crossAx val="288763384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="297"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="371191704"/>
+        <c:axId val="288763384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1337,7 +1332,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1404,7 +1398,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="289031360"/>
+        <c:crossAx val="288222616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2333,8 +2327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2357,67 +2351,67 @@
         <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>28</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>29</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>30</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>31</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>32</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>33</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>34</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>35</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>36</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>37</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>38</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>39</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>40</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>41</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>42</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>43</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>44</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
@@ -5550,7 +5544,7 @@
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>14</v>
@@ -5741,8 +5735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5755,69 +5749,69 @@
         <v>24</v>
       </c>
       <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>27</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>28</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>29</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>30</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>31</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>32</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>33</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>35</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>36</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>37</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>38</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>39</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>40</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>41</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>42</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>43</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>44</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" t="e">
         <f>AVERAGE(H2:Q2)</f>
@@ -5833,7 +5827,7 @@
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B5" si="0">AVERAGE(H3:Q3)</f>
@@ -5909,7 +5903,7 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" t="e">
         <f t="shared" si="0"/>
@@ -5925,23 +5919,53 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="C5" t="e">
+      <c r="C5">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>112.7</v>
       </c>
       <c r="E5" t="s">
         <v>3</v>
       </c>
+      <c r="S5">
+        <v>121</v>
+      </c>
+      <c r="T5">
+        <v>119</v>
+      </c>
+      <c r="U5">
+        <v>123</v>
+      </c>
+      <c r="V5">
+        <v>109</v>
+      </c>
+      <c r="W5">
+        <v>97</v>
+      </c>
+      <c r="X5">
+        <v>111</v>
+      </c>
+      <c r="Y5">
+        <v>112</v>
+      </c>
+      <c r="Z5">
+        <v>105</v>
+      </c>
+      <c r="AA5">
+        <v>112</v>
+      </c>
+      <c r="AB5">
+        <v>118</v>
+      </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" t="e">
         <f>AVERAGE(H6:Q6)</f>
@@ -5959,43 +5983,157 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:AB6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>23</v>
       </c>
       <c r="C1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S1" t="s">
+        <v>35</v>
+      </c>
+      <c r="T1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>45</v>
+      </c>
+      <c r="B2" t="e">
+        <f>AVERAGE(H2:Q2)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C2" t="e">
+        <f>AVERAGE(S2:AB2)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="e">
+        <f t="shared" ref="B3:B5" si="0">AVERAGE(H3:Q3)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C3" t="e">
+        <f t="shared" ref="C3:C5" si="1">AVERAGE(S3:AB3)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="E3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C4" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="E4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="E5" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="e">
+        <f>AVERAGE(H6:Q6)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C6" t="e">
+        <f>AVERAGE(S6:AB6)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added some -O0 results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="75">
   <si>
     <t># Cells</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>PH(0) 10</t>
+  </si>
+  <si>
+    <t>TSN</t>
   </si>
 </sst>
 </file>
@@ -281,12 +284,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5802,10 +5806,13 @@
   <dimension ref="A1:AN6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
@@ -5910,37 +5917,97 @@
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" t="e">
+        <v>74</v>
+      </c>
+      <c r="B2" s="3" t="e">
         <f>AVERAGE(I2:R2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C2" t="e">
+      <c r="C2" s="3">
         <f>AVERAGE(T2:AC2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D2" t="e">
+        <v>118.8</v>
+      </c>
+      <c r="D2" s="3">
         <f>AVERAGE(AE2:AN2)</f>
-        <v>#DIV/0!</v>
+        <v>316.10000000000002</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="T2">
+        <v>126</v>
+      </c>
+      <c r="U2">
+        <v>124</v>
+      </c>
+      <c r="V2">
+        <v>128</v>
+      </c>
+      <c r="W2">
+        <v>115</v>
+      </c>
+      <c r="X2">
+        <v>115</v>
+      </c>
+      <c r="Y2">
+        <v>123</v>
+      </c>
+      <c r="Z2">
+        <v>115</v>
+      </c>
+      <c r="AA2">
+        <v>128</v>
+      </c>
+      <c r="AB2">
+        <v>102</v>
+      </c>
+      <c r="AC2">
+        <v>112</v>
+      </c>
+      <c r="AE2">
+        <v>313</v>
+      </c>
+      <c r="AF2">
+        <v>321</v>
+      </c>
+      <c r="AG2">
+        <v>333</v>
+      </c>
+      <c r="AH2">
+        <v>314</v>
+      </c>
+      <c r="AI2">
+        <v>319</v>
+      </c>
+      <c r="AJ2">
+        <v>311</v>
+      </c>
+      <c r="AK2">
+        <v>312</v>
+      </c>
+      <c r="AL2">
+        <v>310</v>
+      </c>
+      <c r="AM2">
+        <v>312</v>
+      </c>
+      <c r="AN2">
+        <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>46</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <f t="shared" ref="B3:B5" si="0">AVERAGE(I3:R3)</f>
         <v>14253.6</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <f t="shared" ref="C3:C5" si="1">AVERAGE(T3:AC3)</f>
         <v>713.4</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <f t="shared" ref="D3:D6" si="2">AVERAGE(AE3:AN3)</f>
         <v>1996.9</v>
       </c>
@@ -6042,15 +6109,15 @@
       <c r="A4" t="s">
         <v>47</v>
       </c>
-      <c r="B4" t="e">
+      <c r="B4" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="C4" t="e">
+      <c r="C4" s="3" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="D4" t="e">
+      <c r="D4" s="3" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -6062,17 +6129,17 @@
       <c r="A5" t="s">
         <v>48</v>
       </c>
-      <c r="B5" t="e">
+      <c r="B5" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <f t="shared" si="1"/>
         <v>112.7</v>
       </c>
-      <c r="D5" t="e">
+      <c r="D5" s="3">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>248.8</v>
       </c>
       <c r="F5" t="s">
         <v>3</v>
@@ -6106,23 +6173,53 @@
       </c>
       <c r="AC5">
         <v>118</v>
+      </c>
+      <c r="AE5">
+        <v>252</v>
+      </c>
+      <c r="AF5">
+        <v>252</v>
+      </c>
+      <c r="AG5">
+        <v>249</v>
+      </c>
+      <c r="AH5">
+        <v>252</v>
+      </c>
+      <c r="AI5">
+        <v>251</v>
+      </c>
+      <c r="AJ5">
+        <v>244</v>
+      </c>
+      <c r="AK5">
+        <v>252</v>
+      </c>
+      <c r="AL5">
+        <v>243</v>
+      </c>
+      <c r="AM5">
+        <v>251</v>
+      </c>
+      <c r="AN5">
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>49</v>
       </c>
-      <c r="B6" t="e">
+      <c r="B6" s="3" t="e">
         <f>AVERAGE(I6:R6)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <f>AVERAGE(T6:AC6)</f>
         <v>206.9</v>
       </c>
-      <c r="D6" t="e">
+      <c r="D6" s="3">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>503.5</v>
       </c>
       <c r="T6">
         <v>214</v>
@@ -6154,9 +6251,40 @@
       <c r="AC6">
         <v>208</v>
       </c>
+      <c r="AE6">
+        <v>506</v>
+      </c>
+      <c r="AF6">
+        <v>516</v>
+      </c>
+      <c r="AG6">
+        <v>511</v>
+      </c>
+      <c r="AH6">
+        <v>501</v>
+      </c>
+      <c r="AI6">
+        <v>487</v>
+      </c>
+      <c r="AJ6">
+        <v>492</v>
+      </c>
+      <c r="AK6">
+        <v>502</v>
+      </c>
+      <c r="AL6">
+        <v>506</v>
+      </c>
+      <c r="AM6">
+        <v>515</v>
+      </c>
+      <c r="AN6">
+        <v>499</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added the final Piha results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1227,11 +1227,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="126784920"/>
-        <c:axId val="126785312"/>
+        <c:axId val="177704064"/>
+        <c:axId val="179818760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="126784920"/>
+        <c:axId val="177704064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2000"/>
@@ -1345,13 +1345,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="126785312"/>
+        <c:crossAx val="179818760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="297"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="126785312"/>
+        <c:axId val="179818760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1468,7 +1468,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="126784920"/>
+        <c:crossAx val="177704064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5806,7 +5806,7 @@
   <dimension ref="A1:AN6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="AO4" sqref="AO4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6113,16 +6113,76 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="C4" s="3" t="e">
+      <c r="C4" s="3">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D4" s="3" t="e">
+        <v>147</v>
+      </c>
+      <c r="D4" s="3">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>334.9</v>
       </c>
       <c r="F4" t="s">
         <v>2</v>
+      </c>
+      <c r="T4">
+        <v>145</v>
+      </c>
+      <c r="U4">
+        <v>149</v>
+      </c>
+      <c r="V4">
+        <v>144</v>
+      </c>
+      <c r="W4">
+        <v>150</v>
+      </c>
+      <c r="X4">
+        <v>145</v>
+      </c>
+      <c r="Y4">
+        <v>146</v>
+      </c>
+      <c r="Z4">
+        <v>146</v>
+      </c>
+      <c r="AA4">
+        <v>152</v>
+      </c>
+      <c r="AB4">
+        <v>146</v>
+      </c>
+      <c r="AC4">
+        <v>147</v>
+      </c>
+      <c r="AE4">
+        <v>330</v>
+      </c>
+      <c r="AF4">
+        <v>332</v>
+      </c>
+      <c r="AG4">
+        <v>348</v>
+      </c>
+      <c r="AH4">
+        <v>339</v>
+      </c>
+      <c r="AI4">
+        <v>343</v>
+      </c>
+      <c r="AJ4">
+        <v>336</v>
+      </c>
+      <c r="AK4">
+        <v>329</v>
+      </c>
+      <c r="AL4">
+        <v>331</v>
+      </c>
+      <c r="AM4">
+        <v>330</v>
+      </c>
+      <c r="AN4">
+        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated all results to MSVC++ compiler data
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1227,11 +1227,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="177704064"/>
-        <c:axId val="179818760"/>
+        <c:axId val="244914960"/>
+        <c:axId val="244915352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="177704064"/>
+        <c:axId val="244914960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2000"/>
@@ -1345,13 +1345,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="179818760"/>
+        <c:crossAx val="244915352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="297"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="179818760"/>
+        <c:axId val="244915352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1468,7 +1468,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177704064"/>
+        <c:crossAx val="244914960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5806,7 +5806,7 @@
   <dimension ref="A1:AN6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AO4" sqref="AO4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5925,74 +5925,74 @@
       </c>
       <c r="C2" s="3">
         <f>AVERAGE(T2:AC2)</f>
-        <v>118.8</v>
+        <v>118.7</v>
       </c>
       <c r="D2" s="3">
         <f>AVERAGE(AE2:AN2)</f>
-        <v>316.10000000000002</v>
+        <v>285.89999999999998</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>22</v>
       </c>
       <c r="T2">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="U2">
+        <v>88</v>
+      </c>
+      <c r="V2">
+        <v>117</v>
+      </c>
+      <c r="W2">
+        <v>106</v>
+      </c>
+      <c r="X2">
         <v>124</v>
       </c>
-      <c r="V2">
-        <v>128</v>
-      </c>
-      <c r="W2">
-        <v>115</v>
-      </c>
-      <c r="X2">
-        <v>115</v>
-      </c>
       <c r="Y2">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="Z2">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="AA2">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="AB2">
-        <v>102</v>
+        <v>133</v>
       </c>
       <c r="AC2">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="AE2">
-        <v>313</v>
+        <v>285</v>
       </c>
       <c r="AF2">
-        <v>321</v>
+        <v>263</v>
       </c>
       <c r="AG2">
-        <v>333</v>
+        <v>286</v>
       </c>
       <c r="AH2">
-        <v>314</v>
+        <v>288</v>
       </c>
       <c r="AI2">
-        <v>319</v>
+        <v>275</v>
       </c>
       <c r="AJ2">
-        <v>311</v>
+        <v>295</v>
       </c>
       <c r="AK2">
-        <v>312</v>
+        <v>276</v>
       </c>
       <c r="AL2">
-        <v>310</v>
+        <v>289</v>
       </c>
       <c r="AM2">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="AN2">
-        <v>316</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.25">
@@ -6000,109 +6000,109 @@
         <v>46</v>
       </c>
       <c r="B3" s="3">
-        <f t="shared" ref="B3:B5" si="0">AVERAGE(I3:R3)</f>
-        <v>14253.6</v>
+        <f t="shared" ref="B3:B6" si="0">AVERAGE(I3:R3)</f>
+        <v>13709.3</v>
       </c>
       <c r="C3" s="3">
-        <f t="shared" ref="C3:C5" si="1">AVERAGE(T3:AC3)</f>
-        <v>713.4</v>
+        <f t="shared" ref="C3:C4" si="1">AVERAGE(T3:AC3)</f>
+        <v>676.2</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:D6" si="2">AVERAGE(AE3:AN3)</f>
-        <v>1996.9</v>
+        <f t="shared" ref="D3:D4" si="2">AVERAGE(AE3:AN3)</f>
+        <v>1644.9</v>
       </c>
       <c r="F3" t="s">
         <v>1</v>
       </c>
       <c r="I3">
-        <v>14418</v>
+        <v>13873</v>
       </c>
       <c r="J3">
-        <v>14271</v>
+        <v>13626</v>
       </c>
       <c r="K3">
-        <v>14266</v>
+        <v>13756</v>
       </c>
       <c r="L3">
-        <v>14235</v>
+        <v>13757</v>
       </c>
       <c r="M3">
-        <v>14279</v>
+        <v>13636</v>
       </c>
       <c r="N3">
-        <v>14219</v>
+        <v>13795</v>
       </c>
       <c r="O3">
-        <v>14260</v>
+        <v>13593</v>
       </c>
       <c r="P3">
-        <v>14205</v>
+        <v>13639</v>
       </c>
       <c r="Q3">
-        <v>14201</v>
+        <v>13631</v>
       </c>
       <c r="R3">
-        <v>14182</v>
+        <v>13787</v>
       </c>
       <c r="T3">
-        <v>749</v>
+        <v>689</v>
       </c>
       <c r="U3">
-        <v>718</v>
+        <v>678</v>
       </c>
       <c r="V3">
-        <v>702</v>
+        <v>669</v>
       </c>
       <c r="W3">
-        <v>719</v>
+        <v>685</v>
       </c>
       <c r="X3">
-        <v>718</v>
+        <v>662</v>
       </c>
       <c r="Y3">
-        <v>702</v>
+        <v>668</v>
       </c>
       <c r="Z3">
-        <v>718</v>
+        <v>685</v>
       </c>
       <c r="AA3">
-        <v>702</v>
+        <v>670</v>
       </c>
       <c r="AB3">
-        <v>702</v>
+        <v>671</v>
       </c>
       <c r="AC3">
-        <v>704</v>
+        <v>685</v>
       </c>
       <c r="AE3">
-        <v>2022</v>
+        <v>1630</v>
       </c>
       <c r="AF3">
-        <v>1993</v>
+        <v>1653</v>
       </c>
       <c r="AG3">
-        <v>2016</v>
+        <v>1650</v>
       </c>
       <c r="AH3">
-        <v>1998</v>
+        <v>1645</v>
       </c>
       <c r="AI3">
-        <v>2015</v>
+        <v>1663</v>
       </c>
       <c r="AJ3">
-        <v>1985</v>
+        <v>1641</v>
       </c>
       <c r="AK3">
-        <v>1991</v>
+        <v>1638</v>
       </c>
       <c r="AL3">
-        <v>2001</v>
+        <v>1643</v>
       </c>
       <c r="AM3">
-        <v>1973</v>
+        <v>1617</v>
       </c>
       <c r="AN3">
-        <v>1975</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.25">
@@ -6115,74 +6115,74 @@
       </c>
       <c r="C4" s="3">
         <f t="shared" si="1"/>
-        <v>147</v>
+        <v>134.5</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" si="2"/>
-        <v>334.9</v>
+        <v>320.8</v>
       </c>
       <c r="F4" t="s">
         <v>2</v>
       </c>
       <c r="T4">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="U4">
-        <v>149</v>
+        <v>117</v>
       </c>
       <c r="V4">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="W4">
+        <v>143</v>
+      </c>
+      <c r="X4">
+        <v>135</v>
+      </c>
+      <c r="Y4">
+        <v>138</v>
+      </c>
+      <c r="Z4">
+        <v>137</v>
+      </c>
+      <c r="AA4">
+        <v>121</v>
+      </c>
+      <c r="AB4">
+        <v>140</v>
+      </c>
+      <c r="AC4">
         <v>150</v>
       </c>
-      <c r="X4">
-        <v>145</v>
-      </c>
-      <c r="Y4">
-        <v>146</v>
-      </c>
-      <c r="Z4">
-        <v>146</v>
-      </c>
-      <c r="AA4">
-        <v>152</v>
-      </c>
-      <c r="AB4">
-        <v>146</v>
-      </c>
-      <c r="AC4">
-        <v>147</v>
-      </c>
       <c r="AE4">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="AF4">
+        <v>333</v>
+      </c>
+      <c r="AG4">
+        <v>294</v>
+      </c>
+      <c r="AH4">
+        <v>318</v>
+      </c>
+      <c r="AI4">
+        <v>317</v>
+      </c>
+      <c r="AJ4">
+        <v>311</v>
+      </c>
+      <c r="AK4">
+        <v>326</v>
+      </c>
+      <c r="AL4">
+        <v>318</v>
+      </c>
+      <c r="AM4">
         <v>332</v>
       </c>
-      <c r="AG4">
-        <v>348</v>
-      </c>
-      <c r="AH4">
-        <v>339</v>
-      </c>
-      <c r="AI4">
-        <v>343</v>
-      </c>
-      <c r="AJ4">
+      <c r="AN4">
         <v>336</v>
-      </c>
-      <c r="AK4">
-        <v>329</v>
-      </c>
-      <c r="AL4">
-        <v>331</v>
-      </c>
-      <c r="AM4">
-        <v>330</v>
-      </c>
-      <c r="AN4">
-        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.25">
@@ -6194,75 +6194,75 @@
         <v>#DIV/0!</v>
       </c>
       <c r="C5" s="3">
-        <f t="shared" si="1"/>
-        <v>112.7</v>
+        <f>AVERAGE(T5:AC5)</f>
+        <v>100.7</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" si="2"/>
-        <v>248.8</v>
+        <f>AVERAGE(AE5:AN5)</f>
+        <v>255.7</v>
       </c>
       <c r="F5" t="s">
         <v>3</v>
       </c>
       <c r="T5">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="U5">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="V5">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="W5">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X5">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="Y5">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="Z5">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="AA5">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="AB5">
         <v>112</v>
       </c>
       <c r="AC5">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="AE5">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="AF5">
-        <v>252</v>
+        <v>263</v>
       </c>
       <c r="AG5">
-        <v>249</v>
+        <v>269</v>
       </c>
       <c r="AH5">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="AI5">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="AJ5">
-        <v>244</v>
+        <v>257</v>
       </c>
       <c r="AK5">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AL5">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="AM5">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="AN5">
-        <v>242</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.25">
@@ -6270,76 +6270,76 @@
         <v>49</v>
       </c>
       <c r="B6" s="3" t="e">
-        <f>AVERAGE(I6:R6)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C6" s="3">
         <f>AVERAGE(T6:AC6)</f>
-        <v>206.9</v>
+        <v>157</v>
       </c>
       <c r="D6" s="3">
-        <f t="shared" si="2"/>
-        <v>503.5</v>
+        <f>AVERAGE(AE6:AN6)</f>
+        <v>458.7</v>
       </c>
       <c r="T6">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="U6">
-        <v>213</v>
+        <v>144</v>
       </c>
       <c r="V6">
-        <v>210</v>
+        <v>156</v>
       </c>
       <c r="W6">
-        <v>211</v>
+        <v>155</v>
       </c>
       <c r="X6">
-        <v>199</v>
+        <v>156</v>
       </c>
       <c r="Y6">
-        <v>199</v>
+        <v>154</v>
       </c>
       <c r="Z6">
-        <v>207</v>
+        <v>164</v>
       </c>
       <c r="AA6">
-        <v>200</v>
+        <v>165</v>
       </c>
       <c r="AB6">
-        <v>208</v>
+        <v>157</v>
       </c>
       <c r="AC6">
-        <v>208</v>
+        <v>155</v>
       </c>
       <c r="AE6">
-        <v>506</v>
+        <v>482</v>
       </c>
       <c r="AF6">
-        <v>516</v>
+        <v>431</v>
       </c>
       <c r="AG6">
-        <v>511</v>
+        <v>456</v>
       </c>
       <c r="AH6">
-        <v>501</v>
+        <v>456</v>
       </c>
       <c r="AI6">
-        <v>487</v>
+        <v>460</v>
       </c>
       <c r="AJ6">
-        <v>492</v>
+        <v>459</v>
       </c>
       <c r="AK6">
-        <v>502</v>
+        <v>464</v>
       </c>
       <c r="AL6">
-        <v>506</v>
+        <v>455</v>
       </c>
       <c r="AM6">
-        <v>515</v>
+        <v>468</v>
       </c>
       <c r="AN6">
-        <v>499</v>
+        <v>456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed second metric from memory usage (too hard to measure and only massive increase for Heart) to executable size
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -9,14 +9,13 @@
   <sheets>
     <sheet name="Scalability" sheetId="1" r:id="rId1"/>
     <sheet name="Simulation Time" sheetId="2" r:id="rId2"/>
-    <sheet name="Memory Usage" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="75">
   <si>
     <t># Cells</t>
   </si>
@@ -151,9 +150,6 @@
   </si>
   <si>
     <t>PH 10</t>
-  </si>
-  <si>
-    <t>TTS</t>
   </si>
   <si>
     <t>NHC</t>
@@ -1230,11 +1226,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="203008648"/>
-        <c:axId val="203009040"/>
+        <c:axId val="254767920"/>
+        <c:axId val="199621392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="203008648"/>
+        <c:axId val="254767920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2000"/>
@@ -1348,13 +1344,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203009040"/>
+        <c:crossAx val="199621392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="297"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="203009040"/>
+        <c:axId val="199621392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1471,7 +1467,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203008648"/>
+        <c:crossAx val="254767920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2424,7 +2420,7 @@
         <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G1" t="s">
         <v>25</v>
@@ -5617,7 +5613,7 @@
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>14</v>
@@ -5809,7 +5805,7 @@
   <dimension ref="A1:AN13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5822,10 +5818,10 @@
         <v>23</v>
       </c>
       <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
         <v>52</v>
-      </c>
-      <c r="D1" t="s">
-        <v>53</v>
       </c>
       <c r="I1" t="s">
         <v>25</v>
@@ -5858,69 +5854,69 @@
         <v>34</v>
       </c>
       <c r="T1" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1" t="s">
         <v>54</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>55</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>56</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>57</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>58</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>59</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>60</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>61</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>62</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>63</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>64</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>65</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>66</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>67</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>68</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>69</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>70</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>71</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>72</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="3">
         <f>AVERAGE(I2:R2)</f>
@@ -6030,7 +6026,7 @@
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="3">
         <f t="shared" ref="B3:B4" si="0">AVERAGE(I3:R3)</f>
@@ -6140,7 +6136,7 @@
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="3">
         <f t="shared" si="0"/>
@@ -6250,7 +6246,7 @@
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="3">
         <f>AVERAGE(I5:R5)</f>
@@ -6360,7 +6356,7 @@
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="3">
         <f>AVERAGE(I6:R6)</f>
@@ -6467,7 +6463,7 @@
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C9">
         <f>B2/C2</f>
@@ -6522,164 +6518,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O1" t="s">
-        <v>32</v>
-      </c>
-      <c r="P1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S1" t="s">
-        <v>35</v>
-      </c>
-      <c r="T1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V1" t="s">
-        <v>38</v>
-      </c>
-      <c r="W1" t="s">
-        <v>39</v>
-      </c>
-      <c r="X1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" t="e">
-        <f>AVERAGE(H2:Q2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C2" t="e">
-        <f>AVERAGE(S2:AB2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" t="e">
-        <f t="shared" ref="B3:B5" si="0">AVERAGE(H3:Q3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C3" t="e">
-        <f t="shared" ref="C3:C5" si="1">AVERAGE(S3:AB3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C4" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C5" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" t="e">
-        <f>AVERAGE(H6:Q6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C6" t="e">
-        <f>AVERAGE(S6:AB6)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added numbers to the results section
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Scalability" sheetId="1" r:id="rId1"/>
     <sheet name="Simulation Time" sheetId="2" r:id="rId2"/>
+    <sheet name="Executable Size" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="75">
   <si>
     <t># Cells</t>
   </si>
@@ -1226,11 +1227,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="254767920"/>
-        <c:axId val="199621392"/>
+        <c:axId val="170963136"/>
+        <c:axId val="170963528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="254767920"/>
+        <c:axId val="170963136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2000"/>
@@ -1344,13 +1345,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="199621392"/>
+        <c:crossAx val="170963528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="297"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="199621392"/>
+        <c:axId val="170963528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1467,7 +1468,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254767920"/>
+        <c:crossAx val="170963136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5802,10 +5803,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN13"/>
+  <dimension ref="A1:AN15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6514,8 +6515,225 @@
         <v>2.3601482450403313</v>
       </c>
     </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <f>AVERAGE(C9:C13)</f>
+        <v>9.8439930921626111</v>
+      </c>
+      <c r="D15">
+        <f>AVERAGE(D9:D13)</f>
+        <v>3.9528483500609326</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="3">
+        <v>190</v>
+      </c>
+      <c r="C2" s="3">
+        <v>96</v>
+      </c>
+      <c r="D2" s="3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="3">
+        <v>320</v>
+      </c>
+      <c r="C3" s="3">
+        <v>128</v>
+      </c>
+      <c r="D3" s="3">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="3">
+        <v>226</v>
+      </c>
+      <c r="C4" s="3">
+        <v>98</v>
+      </c>
+      <c r="D4" s="3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="3">
+        <v>188</v>
+      </c>
+      <c r="C5" s="3">
+        <v>97</v>
+      </c>
+      <c r="D5" s="3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="3">
+        <v>212</v>
+      </c>
+      <c r="C6" s="3">
+        <v>98</v>
+      </c>
+      <c r="D6" s="3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9">
+        <f>B2/C2</f>
+        <v>1.9791666666666667</v>
+      </c>
+      <c r="D9">
+        <f>B2/D2</f>
+        <v>1.4503816793893129</v>
+      </c>
+      <c r="F9">
+        <f>100*($B2-C2)/B2</f>
+        <v>49.473684210526315</v>
+      </c>
+      <c r="G9">
+        <f>100*($B2-D2)/C2</f>
+        <v>61.458333333333336</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <f>B3/C3</f>
+        <v>2.5</v>
+      </c>
+      <c r="D10">
+        <f>B3/D3</f>
+        <v>0.99071207430340558</v>
+      </c>
+      <c r="F10">
+        <f t="shared" ref="F10:G13" si="0">100*($B3-C3)/B3</f>
+        <v>60</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>-2.34375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <f>B4/C4</f>
+        <v>2.306122448979592</v>
+      </c>
+      <c r="D11">
+        <f>B4/D4</f>
+        <v>1.3865030674846626</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>56.637168141592923</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>64.285714285714292</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <f>B5/C5</f>
+        <v>1.9381443298969072</v>
+      </c>
+      <c r="D12">
+        <f>B5/D5</f>
+        <v>1.4461538461538461</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>48.404255319148938</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>59.793814432989691</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <f>B6/C6</f>
+        <v>2.1632653061224492</v>
+      </c>
+      <c r="D13">
+        <f>B6/D6</f>
+        <v>1.2183908045977012</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>53.773584905660378</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>38.775510204081634</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <f>AVERAGE(C9:C13)</f>
+        <v>2.1773397503331231</v>
+      </c>
+      <c r="D15">
+        <f>AVERAGE(D9:D13)</f>
+        <v>1.2984282943857857</v>
+      </c>
+      <c r="F15">
+        <f>AVERAGE(F9:F13)</f>
+        <v>53.657738515385709</v>
+      </c>
+      <c r="G15">
+        <f>AVERAGE(G9:G13)</f>
+        <v>44.393924451223789</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated execution time graph to be relative to Simulink
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,17 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26207"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathan/git/DATE2016_codegen/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="8600" yWindow="3500" windowWidth="25000" windowHeight="14960" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Scalability" sheetId="1" r:id="rId1"/>
     <sheet name="Simulation Time" sheetId="2" r:id="rId2"/>
     <sheet name="Executable Size" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -284,13 +294,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -311,7 +322,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-NZ"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -428,184 +439,184 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
-                  <c:v>33</c:v>
+                  <c:v>33.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>66</c:v>
+                  <c:v>66.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>99</c:v>
+                  <c:v>99.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>132</c:v>
+                  <c:v>132.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>165</c:v>
+                  <c:v>165.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>198</c:v>
+                  <c:v>198.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>231</c:v>
+                  <c:v>231.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>264</c:v>
+                  <c:v>264.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>297</c:v>
+                  <c:v>297.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>330</c:v>
+                  <c:v>330.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>363</c:v>
+                  <c:v>363.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>396</c:v>
+                  <c:v>396.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>429</c:v>
+                  <c:v>429.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>462</c:v>
+                  <c:v>462.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>495</c:v>
+                  <c:v>495.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>528</c:v>
+                  <c:v>528.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>561</c:v>
+                  <c:v>561.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>594</c:v>
+                  <c:v>594.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>627</c:v>
+                  <c:v>627.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>660</c:v>
+                  <c:v>660.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>693</c:v>
+                  <c:v>693.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>726</c:v>
+                  <c:v>726.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>759</c:v>
+                  <c:v>759.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>792</c:v>
+                  <c:v>792.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>825</c:v>
+                  <c:v>825.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>858</c:v>
+                  <c:v>858.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>891</c:v>
+                  <c:v>891.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>924</c:v>
+                  <c:v>924.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>957</c:v>
+                  <c:v>957.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>990</c:v>
+                  <c:v>990.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1023</c:v>
+                  <c:v>1023.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1056</c:v>
+                  <c:v>1056.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1089</c:v>
+                  <c:v>1089.0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1122</c:v>
+                  <c:v>1122.0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1155</c:v>
+                  <c:v>1155.0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1188</c:v>
+                  <c:v>1188.0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1221</c:v>
+                  <c:v>1221.0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1254</c:v>
+                  <c:v>1254.0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1287</c:v>
+                  <c:v>1287.0</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1320</c:v>
+                  <c:v>1320.0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1353</c:v>
+                  <c:v>1353.0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1386</c:v>
+                  <c:v>1386.0</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1419</c:v>
+                  <c:v>1419.0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1452</c:v>
+                  <c:v>1452.0</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1485</c:v>
+                  <c:v>1485.0</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1518</c:v>
+                  <c:v>1518.0</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1551</c:v>
+                  <c:v>1551.0</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1584</c:v>
+                  <c:v>1584.0</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1617</c:v>
+                  <c:v>1617.0</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1650</c:v>
+                  <c:v>1650.0</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1683</c:v>
+                  <c:v>1683.0</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1716</c:v>
+                  <c:v>1716.0</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1749</c:v>
+                  <c:v>1749.0</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1782</c:v>
+                  <c:v>1782.0</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1815</c:v>
+                  <c:v>1815.0</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1848</c:v>
+                  <c:v>1848.0</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1881</c:v>
+                  <c:v>1881.0</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1914</c:v>
+                  <c:v>1914.0</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1947</c:v>
+                  <c:v>1947.0</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1980</c:v>
+                  <c:v>1980.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -617,40 +628,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
-                  <c:v>0.73199999999999998</c:v>
+                  <c:v>0.732</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7189999999999994</c:v>
+                  <c:v>1.718999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.8380000000000005</c:v>
+                  <c:v>2.838</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.6160000000000014</c:v>
+                  <c:v>4.616000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.2849999999999993</c:v>
+                  <c:v>7.284999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.095000000000001</c:v>
+                  <c:v>11.095</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16.411999999999999</c:v>
+                  <c:v>16.412</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23.025000000000002</c:v>
+                  <c:v>23.025</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>31.122999999999998</c:v>
+                  <c:v>31.123</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>38.424999999999997</c:v>
+                  <c:v>38.425</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45.940999999999995</c:v>
+                  <c:v>45.941</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>52.601999999999997</c:v>
+                  <c:v>52.602</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>59.35799999999999</c:v>
@@ -659,106 +670,106 @@
                   <c:v>65.38000000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>71.759999999999991</c:v>
+                  <c:v>71.76</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>77.626000000000005</c:v>
+                  <c:v>77.626</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>81.759</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>84.864000000000019</c:v>
+                  <c:v>84.86400000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>91.266999999999996</c:v>
+                  <c:v>91.267</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>96.097999999999999</c:v>
+                  <c:v>96.098</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>100.40200000000002</c:v>
+                  <c:v>100.402</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>104.66100000000002</c:v>
+                  <c:v>104.661</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>112.742</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>118.29400000000001</c:v>
+                  <c:v>118.294</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>121.571</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>127.53000000000002</c:v>
+                  <c:v>127.53</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>131.96099999999998</c:v>
+                  <c:v>131.961</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>139.089</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>146.16999999999999</c:v>
+                  <c:v>146.17</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>148.38600000000002</c:v>
+                  <c:v>148.386</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>165.96800000000002</c:v>
+                  <c:v>165.968</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>166.64600000000002</c:v>
+                  <c:v>166.646</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>170.52499999999998</c:v>
+                  <c:v>170.525</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>172.89400000000001</c:v>
+                  <c:v>172.894</c:v>
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>184.298</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>182.97199999999998</c:v>
+                  <c:v>182.972</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>194.17299999999997</c:v>
+                  <c:v>194.173</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>206.45100000000002</c:v>
+                  <c:v>206.451</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>224.84299999999999</c:v>
+                  <c:v>224.843</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>219.429</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>232.77699999999996</c:v>
+                  <c:v>232.777</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>246.34100000000004</c:v>
+                  <c:v>246.341</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>256.27499999999998</c:v>
+                  <c:v>256.275</c:v>
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>273.5</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>268.46000000000004</c:v>
+                  <c:v>268.46</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>296.25999999999993</c:v>
+                  <c:v>296.2599999999999</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>304.48099999999999</c:v>
+                  <c:v>304.481</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>328.75600000000003</c:v>
+                  <c:v>328.756</c:v>
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>341.89</c:v>
@@ -767,34 +778,34 @@
                   <c:v>383.59</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>390.31299999999999</c:v>
+                  <c:v>390.313</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>395.11700000000008</c:v>
+                  <c:v>395.1170000000001</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>436.78800000000001</c:v>
+                  <c:v>436.788</c:v>
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>487.471</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>476.83000000000004</c:v>
+                  <c:v>476.83</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>485.89299999999992</c:v>
+                  <c:v>485.8929999999999</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>537.22299999999996</c:v>
+                  <c:v>537.223</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>543.78600000000006</c:v>
+                  <c:v>543.786</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>564.42499999999995</c:v>
+                  <c:v>564.425</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>608.72700000000009</c:v>
+                  <c:v>608.7270000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -846,184 +857,184 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
-                  <c:v>33</c:v>
+                  <c:v>33.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>66</c:v>
+                  <c:v>66.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>99</c:v>
+                  <c:v>99.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>132</c:v>
+                  <c:v>132.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>165</c:v>
+                  <c:v>165.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>198</c:v>
+                  <c:v>198.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>231</c:v>
+                  <c:v>231.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>264</c:v>
+                  <c:v>264.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>297</c:v>
+                  <c:v>297.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>330</c:v>
+                  <c:v>330.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>363</c:v>
+                  <c:v>363.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>396</c:v>
+                  <c:v>396.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>429</c:v>
+                  <c:v>429.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>462</c:v>
+                  <c:v>462.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>495</c:v>
+                  <c:v>495.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>528</c:v>
+                  <c:v>528.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>561</c:v>
+                  <c:v>561.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>594</c:v>
+                  <c:v>594.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>627</c:v>
+                  <c:v>627.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>660</c:v>
+                  <c:v>660.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>693</c:v>
+                  <c:v>693.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>726</c:v>
+                  <c:v>726.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>759</c:v>
+                  <c:v>759.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>792</c:v>
+                  <c:v>792.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>825</c:v>
+                  <c:v>825.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>858</c:v>
+                  <c:v>858.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>891</c:v>
+                  <c:v>891.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>924</c:v>
+                  <c:v>924.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>957</c:v>
+                  <c:v>957.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>990</c:v>
+                  <c:v>990.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1023</c:v>
+                  <c:v>1023.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1056</c:v>
+                  <c:v>1056.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1089</c:v>
+                  <c:v>1089.0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1122</c:v>
+                  <c:v>1122.0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1155</c:v>
+                  <c:v>1155.0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1188</c:v>
+                  <c:v>1188.0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1221</c:v>
+                  <c:v>1221.0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1254</c:v>
+                  <c:v>1254.0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1287</c:v>
+                  <c:v>1287.0</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1320</c:v>
+                  <c:v>1320.0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1353</c:v>
+                  <c:v>1353.0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1386</c:v>
+                  <c:v>1386.0</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1419</c:v>
+                  <c:v>1419.0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1452</c:v>
+                  <c:v>1452.0</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1485</c:v>
+                  <c:v>1485.0</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1518</c:v>
+                  <c:v>1518.0</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1551</c:v>
+                  <c:v>1551.0</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1584</c:v>
+                  <c:v>1584.0</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1617</c:v>
+                  <c:v>1617.0</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1650</c:v>
+                  <c:v>1650.0</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1683</c:v>
+                  <c:v>1683.0</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1716</c:v>
+                  <c:v>1716.0</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1749</c:v>
+                  <c:v>1749.0</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1782</c:v>
+                  <c:v>1782.0</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1815</c:v>
+                  <c:v>1815.0</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1848</c:v>
+                  <c:v>1848.0</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1881</c:v>
+                  <c:v>1881.0</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1914</c:v>
+                  <c:v>1914.0</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1947</c:v>
+                  <c:v>1947.0</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1980</c:v>
+                  <c:v>1980.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1038,181 +1049,181 @@
                   <c:v>8.043000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.091000000000001</c:v>
+                  <c:v>20.091</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35.335999999999999</c:v>
+                  <c:v>35.336</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50.319000000000003</c:v>
+                  <c:v>50.319</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>65.372</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>83.053000000000011</c:v>
+                  <c:v>83.05300000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>98.698000000000008</c:v>
+                  <c:v>98.69800000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>112.28900000000002</c:v>
+                  <c:v>112.289</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>126.44799999999998</c:v>
+                  <c:v>126.448</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1227,15 +1238,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="170963136"/>
-        <c:axId val="170963528"/>
+        <c:axId val="2142003408"/>
+        <c:axId val="2142011472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="170963136"/>
+        <c:axId val="2142003408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="2000"/>
-          <c:min val="33"/>
+          <c:max val="2000.0"/>
+          <c:min val="33.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1345,13 +1356,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="170963528"/>
+        <c:crossAx val="2142011472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="297"/>
+        <c:majorUnit val="297.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="170963528"/>
+        <c:axId val="2142011472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1468,7 +1479,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="170963136"/>
+        <c:crossAx val="2142003408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2397,11 +2408,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA76"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
@@ -2410,7 +2421,7 @@
     <col min="27" max="27" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2484,7 +2495,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>33</v>
       </c>
@@ -2561,7 +2572,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>66</v>
       </c>
@@ -2638,7 +2649,7 @@
         <v>1.56</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>99</v>
       </c>
@@ -2715,7 +2726,7 @@
         <v>2.96</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>132</v>
       </c>
@@ -2792,7 +2803,7 @@
         <v>4.37</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>165</v>
       </c>
@@ -2869,7 +2880,7 @@
         <v>7.18</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>198</v>
       </c>
@@ -2946,7 +2957,7 @@
         <v>11.080000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>231</v>
       </c>
@@ -3023,7 +3034,7 @@
         <v>16.54</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>264</v>
       </c>
@@ -3100,7 +3111,7 @@
         <v>22.93</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>297</v>
       </c>
@@ -3177,7 +3188,7 @@
         <v>31.36</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>330</v>
       </c>
@@ -3224,7 +3235,7 @@
         <v>38.380000000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>363</v>
       </c>
@@ -3271,7 +3282,7 @@
         <v>46.02</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>396</v>
       </c>
@@ -3318,7 +3329,7 @@
         <v>53.35</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>429</v>
       </c>
@@ -3365,7 +3376,7 @@
         <v>59.75</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>462</v>
       </c>
@@ -3412,7 +3423,7 @@
         <v>65.209999999999994</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>495</v>
       </c>
@@ -3459,7 +3470,7 @@
         <v>71.289999999999992</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>528</v>
       </c>
@@ -3506,7 +3517,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>561</v>
       </c>
@@ -3553,7 +3564,7 @@
         <v>81.59</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>594</v>
       </c>
@@ -3600,7 +3611,7 @@
         <v>84.860000000000014</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>627</v>
       </c>
@@ -3647,7 +3658,7 @@
         <v>92.05</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>660</v>
       </c>
@@ -3694,7 +3705,7 @@
         <v>94.85</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>693</v>
       </c>
@@ -3741,7 +3752,7 @@
         <v>103.27</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>726</v>
       </c>
@@ -3788,7 +3799,7 @@
         <v>104.68</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>759</v>
       </c>
@@ -3835,7 +3846,7 @@
         <v>115.60000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>792</v>
       </c>
@@ -3882,7 +3893,7 @@
         <v>121.52</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>825</v>
       </c>
@@ -3929,7 +3940,7 @@
         <v>120.9</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>858</v>
       </c>
@@ -3976,7 +3987,7 @@
         <v>126.67</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>891</v>
       </c>
@@ -4023,7 +4034,7 @@
         <v>131.98000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>924</v>
       </c>
@@ -4070,7 +4081,7 @@
         <v>137.28</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>957</v>
       </c>
@@ -4117,7 +4128,7 @@
         <v>146.47999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>990</v>
       </c>
@@ -4164,7 +4175,7 @@
         <v>147.88999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1023</v>
       </c>
@@ -4211,7 +4222,7 @@
         <v>165.2</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1056</v>
       </c>
@@ -4258,7 +4269,7 @@
         <v>168.64000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1089</v>
       </c>
@@ -4305,7 +4316,7 @@
         <v>170.82</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1122</v>
       </c>
@@ -4352,7 +4363,7 @@
         <v>174.41</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1155</v>
       </c>
@@ -4399,7 +4410,7 @@
         <v>184.86</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1188</v>
       </c>
@@ -4446,7 +4457,7 @@
         <v>183.29999999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1221</v>
       </c>
@@ -4493,7 +4504,7 @@
         <v>195.78</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1254</v>
       </c>
@@ -4540,7 +4551,7 @@
         <v>203.27</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1287</v>
       </c>
@@ -4587,7 +4598,7 @@
         <v>224.17000000000002</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1320</v>
       </c>
@@ -4634,7 +4645,7 @@
         <v>223.70000000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1353</v>
       </c>
@@ -4681,7 +4692,7 @@
         <v>229.95000000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1386</v>
       </c>
@@ -4728,7 +4739,7 @@
         <v>249.13</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1419</v>
       </c>
@@ -4775,7 +4786,7 @@
         <v>256.46000000000004</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1452</v>
       </c>
@@ -4822,7 +4833,7 @@
         <v>276.74</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1485</v>
       </c>
@@ -4869,7 +4880,7 @@
         <v>274.87</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1518</v>
       </c>
@@ -4916,7 +4927,7 @@
         <v>293.75</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1551</v>
       </c>
@@ -4963,7 +4974,7 @@
         <v>299.84000000000003</v>
       </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1584</v>
       </c>
@@ -5010,7 +5021,7 @@
         <v>329.47</v>
       </c>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>1617</v>
       </c>
@@ -5057,7 +5068,7 @@
         <v>339.77</v>
       </c>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1650</v>
       </c>
@@ -5104,7 +5115,7 @@
         <v>370.66</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>1683</v>
       </c>
@@ -5151,7 +5162,7 @@
         <v>392.18000000000006</v>
       </c>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>1716</v>
       </c>
@@ -5198,7 +5209,7 @@
         <v>394.21</v>
       </c>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>1749</v>
       </c>
@@ -5245,7 +5256,7 @@
         <v>435.88</v>
       </c>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>1782</v>
       </c>
@@ -5292,7 +5303,7 @@
         <v>494.68000000000006</v>
       </c>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1815</v>
       </c>
@@ -5339,7 +5350,7 @@
         <v>490.93000000000006</v>
       </c>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>1848</v>
       </c>
@@ -5386,7 +5397,7 @@
         <v>490.46</v>
       </c>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>1881</v>
       </c>
@@ -5433,7 +5444,7 @@
         <v>549.77</v>
       </c>
     </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>1914</v>
       </c>
@@ -5480,7 +5491,7 @@
         <v>545.69000000000005</v>
       </c>
     </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1947</v>
       </c>
@@ -5527,7 +5538,7 @@
         <v>558.64</v>
       </c>
     </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>1980</v>
       </c>
@@ -5574,12 +5585,12 @@
         <v>607.15000000000009</v>
       </c>
     </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>1</v>
       </c>
@@ -5590,7 +5601,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>2</v>
       </c>
@@ -5601,7 +5612,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>3</v>
       </c>
@@ -5612,7 +5623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>50</v>
       </c>
@@ -5629,7 +5640,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>4</v>
       </c>
@@ -5677,7 +5688,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B72" s="1" t="s">
         <v>7</v>
       </c>
@@ -5713,7 +5724,7 @@
         <v>1017632</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
       <c r="G73" s="1" t="s">
         <v>16</v>
       </c>
@@ -5739,7 +5750,7 @@
         <v>127238</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
       <c r="R74" s="1" t="s">
         <v>16</v>
       </c>
@@ -5748,7 +5759,7 @@
         <v>1145142</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>16</v>
       </c>
@@ -5771,7 +5782,7 @@
         <v>8388608</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>19</v>
       </c>
@@ -5805,16 +5816,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="5" width="9.140625" customWidth="1"/>
+    <col min="4" max="5" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>23</v>
       </c>
@@ -5915,7 +5926,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -6025,7 +6036,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -6135,7 +6146,7 @@
         <v>1669</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -6245,7 +6256,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -6355,7 +6366,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -6462,7 +6473,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>74</v>
       </c>
@@ -6475,7 +6486,7 @@
         <v>2.5225603357817423</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
       <c r="C10">
         <f>B3/C3</f>
         <v>20.274031351671102</v>
@@ -6485,7 +6496,7 @@
         <v>8.3344276247796216</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
       <c r="C11">
         <f>B4/C4</f>
         <v>10.060966542750929</v>
@@ -6494,8 +6505,20 @@
         <f>B4/D4</f>
         <v>4.2182044887780545</v>
       </c>
-    </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="G11" s="4">
+        <f>B2/$B2</f>
+        <v>1</v>
+      </c>
+      <c r="H11" s="4">
+        <f t="shared" ref="H11:I11" si="3">C2/$B2</f>
+        <v>0.16458679977814752</v>
+      </c>
+      <c r="I11" s="4">
+        <f t="shared" si="3"/>
+        <v>0.39642262895174701</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
       <c r="C12">
         <f>B5/C5</f>
         <v>5.9136047666335649</v>
@@ -6504,8 +6527,20 @@
         <f>B5/D5</f>
         <v>2.3289010559249119</v>
       </c>
-    </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="G12" s="4">
+        <f t="shared" ref="G12:G15" si="4">B3/$B3</f>
+        <v>1</v>
+      </c>
+      <c r="H12" s="4">
+        <f t="shared" ref="H12:H15" si="5">C3/$B3</f>
+        <v>4.9324181395111355E-2</v>
+      </c>
+      <c r="I12" s="4">
+        <f t="shared" ref="I12:I15" si="6">D3/$B3</f>
+        <v>0.11998424427213644</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
       <c r="C13">
         <f>B6/C6</f>
         <v>6.8955414012738849</v>
@@ -6514,8 +6549,34 @@
         <f>B6/D6</f>
         <v>2.3601482450403313</v>
       </c>
-    </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="G13" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="H13" s="4">
+        <f t="shared" si="5"/>
+        <v>9.9394028968371267E-2</v>
+      </c>
+      <c r="I13" s="4">
+        <f t="shared" si="6"/>
+        <v>0.2370676913981673</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="G14" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="H14" s="4">
+        <f t="shared" si="5"/>
+        <v>0.16910159529806884</v>
+      </c>
+      <c r="I14" s="4">
+        <f t="shared" si="6"/>
+        <v>0.42938706968933665</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
       <c r="C15">
         <f>AVERAGE(C9:C13)</f>
         <v>9.8439930921626111</v>
@@ -6523,6 +6584,18 @@
       <c r="D15">
         <f>AVERAGE(D9:D13)</f>
         <v>3.9528483500609326</v>
+      </c>
+      <c r="G15" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="H15" s="4">
+        <f t="shared" si="5"/>
+        <v>0.14502124515056347</v>
+      </c>
+      <c r="I15" s="4">
+        <f t="shared" si="6"/>
+        <v>0.42370219841123224</v>
       </c>
     </row>
   </sheetData>
@@ -6535,13 +6608,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>23</v>
       </c>
@@ -6552,7 +6625,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -6566,7 +6639,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -6580,7 +6653,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -6594,7 +6667,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -6608,7 +6681,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -6622,7 +6695,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>74</v>
       </c>
@@ -6643,7 +6716,7 @@
         <v>61.458333333333336</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C10">
         <f>B3/C3</f>
         <v>2.5</v>
@@ -6661,7 +6734,7 @@
         <v>-2.34375</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C11">
         <f>B4/C4</f>
         <v>2.306122448979592</v>
@@ -6679,7 +6752,7 @@
         <v>64.285714285714292</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C12">
         <f>B5/C5</f>
         <v>1.9381443298969072</v>
@@ -6697,7 +6770,7 @@
         <v>59.793814432989691</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C13">
         <f>B6/C6</f>
         <v>2.1632653061224492</v>
@@ -6715,7 +6788,7 @@
         <v>38.775510204081634</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C15">
         <f>AVERAGE(C9:C13)</f>
         <v>2.1773397503331231</v>

</xml_diff>